<commit_message>
new menu with steps
</commit_message>
<xml_diff>
--- a/menu.xlsx
+++ b/menu.xlsx
@@ -8,137 +8,175 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bahri\OneDrive - UTS\Desktop\Uni\1\Python\Coffee Menu API\Coffee-Menu-with-API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C0A6A8-0193-4F04-8745-7D40100B9867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81887D47-2FA3-4458-9845-8154EE42EDDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
+  <si>
+    <t>drink</t>
+  </si>
+  <si>
+    <t>price_small</t>
+  </si>
+  <si>
+    <t>price_medium</t>
+  </si>
+  <si>
+    <t>price_large</t>
+  </si>
   <si>
     <t>Espresso</t>
   </si>
   <si>
+    <t>Use 7-9 grams for a single shot or 14-18 grams for a double shot.</t>
+  </si>
+  <si>
+    <t>Brew the espresso shot according to the desired strength and volume.</t>
+  </si>
+  <si>
     <t>Latte</t>
   </si>
   <si>
+    <t>Pull a single shot of espresso (30 ml) into a cup.</t>
+  </si>
+  <si>
+    <t>Steam 200 ml of milk to 65°C, creating a creamy microfoam.</t>
+  </si>
+  <si>
+    <t>Pour the steamed milk into the espresso, holding back the foam with a spoon. Top with a small amount of foam.</t>
+  </si>
+  <si>
     <t>Cappuccino</t>
   </si>
   <si>
+    <t>Steam 150 ml of milk to 65°C, creating a generous amount of foam.</t>
+  </si>
+  <si>
+    <t>Pour the steamed milk and foam over the espresso, aiming for equal parts espresso, milk, and foam.</t>
+  </si>
+  <si>
     <t>Americano</t>
   </si>
   <si>
+    <t>Pull a single shot of espresso (30 ml).</t>
+  </si>
+  <si>
+    <t>Add 90 ml of hot water to the espresso to reach the desired strength</t>
+  </si>
+  <si>
     <t>Mocha</t>
   </si>
   <si>
+    <t>Combine 20 ml of chocolate syrup with a single shot of espresso (30 ml) in a cup.</t>
+  </si>
+  <si>
+    <t>Steam 200 ml of milk to 65°C.</t>
+  </si>
+  <si>
+    <t>Pour the steamed milk into the chocolate-espresso mixture.</t>
+  </si>
+  <si>
+    <t>Top with whipped cream and drizzle with additional chocolate syrup if desired.</t>
+  </si>
+  <si>
     <t>Flat White</t>
   </si>
   <si>
+    <t>Pull a double shot of espresso (60 ml).</t>
+  </si>
+  <si>
+    <t>Steam 150 ml of milk to 65°C, creating a fine microfoam.</t>
+  </si>
+  <si>
+    <t>Pour the steamed milk over the espresso, ensuring a smooth texture with a thin layer of microfoam on top.</t>
+  </si>
+  <si>
     <t>Long Black</t>
   </si>
   <si>
+    <t>Fill a cup with 90-120 ml of hot water.</t>
+  </si>
+  <si>
+    <t>Pour the espresso over the hot water to preserve the crema.</t>
+  </si>
+  <si>
     <t>Short Black</t>
   </si>
   <si>
+    <t>Pull a single shot of espresso (30 ml) into a small cup.</t>
+  </si>
+  <si>
     <t>Chai Latte</t>
   </si>
   <si>
+    <t>Combine 100 ml of chai concentrate with 100 ml of milk.</t>
+  </si>
+  <si>
+    <t>Steam the chai-milk mixture to 65°C.</t>
+  </si>
+  <si>
+    <t>Pour into a cup and optionally sprinkle with cinnamon on top.</t>
+  </si>
+  <si>
     <t>Dirty Chai</t>
   </si>
   <si>
+    <t>Add the espresso shot to the chai latte and mix well.</t>
+  </si>
+  <si>
     <t>Sticky Chai</t>
   </si>
   <si>
-    <t>drink</t>
-  </si>
-  <si>
-    <t>price_small</t>
-  </si>
-  <si>
-    <t>price_medium</t>
-  </si>
-  <si>
-    <t>price_large</t>
-  </si>
-  <si>
-    <t>step_one</t>
-  </si>
-  <si>
-    <t>step_two</t>
-  </si>
-  <si>
-    <t>step_three</t>
-  </si>
-  <si>
-    <t>step_four</t>
-  </si>
-  <si>
-    <t>step_five</t>
-  </si>
-  <si>
-    <t>Use 7-9 grams for a single shot or 14-18 grams for a double shot.</t>
-  </si>
-  <si>
-    <t>Brew the espresso shot according to the desired strength and volume.</t>
-  </si>
-  <si>
-    <t>Pull a single shot of espresso (30 ml) into a cup.</t>
-  </si>
-  <si>
-    <t>Steam 200 ml of milk to 65°C, creating a creamy microfoam.</t>
-  </si>
-  <si>
-    <t>Pour the steamed milk into the espresso, holding back the foam with a spoon. Top with a small amount of foam.</t>
-  </si>
-  <si>
-    <t>Steam 150 ml of milk to 65°C, creating a generous amount of foam.</t>
-  </si>
-  <si>
-    <t>Pour the steamed milk and foam over the espresso, aiming for equal parts espresso, milk, and foam.</t>
-  </si>
-  <si>
-    <t>Pull a single shot of espresso (30 ml).</t>
-  </si>
-  <si>
-    <t>Add 90 ml of hot water to the espresso to reach the desired strength</t>
-  </si>
-  <si>
-    <t>Combine 20 ml of chocolate syrup with a single shot of espresso (30 ml) in a cup.</t>
-  </si>
-  <si>
-    <t>Steam 200 ml of milk to 65°C.</t>
-  </si>
-  <si>
-    <t>Pour the steamed milk into the chocolate-espresso mixture.</t>
-  </si>
-  <si>
-    <t>Top with whipped cream and drizzle with additional chocolate syrup if desired.</t>
-  </si>
-  <si>
-    <t>Pull a double shot of espresso (60 ml).</t>
-  </si>
-  <si>
-    <t>Steam 150 ml of milk to 65°C, creating a fine microfoam.</t>
-  </si>
-  <si>
-    <t>Pour the steamed milk over the espresso, ensuring a smooth texture with a thin layer of microfoam on top.</t>
-  </si>
-  <si>
-    <t>Fill a cup with 90-120 ml of hot water.</t>
-  </si>
-  <si>
-    <t>Pour the espresso over the hot water to preserve the crema.</t>
+    <t>Brew sticky chai tea (loose leaf tea with honey) in a teapot.</t>
+  </si>
+  <si>
+    <t>Steam milk to 65°C.</t>
+  </si>
+  <si>
+    <t>Mix the brewed tea with the steamed milk.</t>
+  </si>
+  <si>
+    <t>Add additional honey for sweetness if desired.</t>
+  </si>
+  <si>
+    <t>step_1</t>
+  </si>
+  <si>
+    <t>step_2</t>
+  </si>
+  <si>
+    <t>step_3</t>
+  </si>
+  <si>
+    <t>step_4</t>
+  </si>
+  <si>
+    <t>step_5</t>
   </si>
 </sst>
 </file>
@@ -478,53 +516,53 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="2" width="10.4609375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="10.3828125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.15234375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.15234375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="60.921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="63.921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="100.4609375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="72.23046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.69140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="60.84375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="63.84375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="100.3828125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="72.3046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="49.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="F1" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="G1" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="H1" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="I1" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.45" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2">
         <v>0.44</v>
@@ -536,15 +574,15 @@
         <v>1.32</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.45" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B3" s="2">
         <v>2.59</v>
@@ -556,18 +594,18 @@
         <v>4.59</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.45" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2">
         <v>3.06</v>
@@ -579,18 +617,18 @@
         <v>5.0599999999999996</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.45" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B5" s="2">
         <v>1.46</v>
@@ -602,15 +640,15 @@
         <v>3.46</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.45" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B6" s="2">
         <v>4.55</v>
@@ -622,21 +660,21 @@
         <v>6.55</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.45" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B7" s="2">
         <v>3.18</v>
@@ -648,18 +686,18 @@
         <v>5.18</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.45" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="B8" s="2">
         <v>1.5</v>
@@ -671,18 +709,18 @@
         <v>3.5</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:9" ht="15.45" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="B9" s="2">
         <v>0.44</v>
@@ -693,10 +731,13 @@
       <c r="D9" s="2">
         <v>1.32</v>
       </c>
+      <c r="E9" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:9" ht="15.45" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B10" s="2">
         <v>2.59</v>
@@ -707,10 +748,19 @@
       <c r="D10" s="2">
         <v>4.59</v>
       </c>
+      <c r="E10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:9" ht="15.45" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="B11" s="2">
         <v>2.99</v>
@@ -721,10 +771,25 @@
       <c r="D11" s="2">
         <v>4.99</v>
       </c>
+      <c r="E11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" ht="15.45" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="B12" s="2">
         <v>2.99</v>
@@ -734,9 +799,314 @@
       </c>
       <c r="D12" s="2">
         <v>4.99</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="fd496924-abde-4845-9207-bf2913a7250c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A47C55F3B8F9A9499A59C314BC32C9D8" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="069ad0183d44500eec8c926aef38c848">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="fd496924-abde-4845-9207-bf2913a7250c" xmlns:ns4="706ff326-42ab-42a4-bae8-1cee897fc7b9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="55994eb0b7e8db7ef86251e0688bf53a" ns3:_="" ns4:_="">
+    <xsd:import namespace="fd496924-abde-4845-9207-bf2913a7250c"/>
+    <xsd:import namespace="706ff326-42ab-42a4-bae8-1cee897fc7b9"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns3:_activity" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns4:SharingHintHash" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceSystemTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="fd496924-abde-4845-9207-bf2913a7250c" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="10" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_activity" ma:index="11" nillable="true" ma:displayName="_activity" ma:hidden="true" ma:internalName="_activity">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="15" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="18" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="19" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="20" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSystemTags" ma:index="21" nillable="true" ma:displayName="MediaServiceSystemTags" ma:hidden="true" ma:internalName="MediaServiceSystemTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="22" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="23" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="706ff326-42ab-42a4-bae8-1cee897fc7b9" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="12" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="13" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SharingHintHash" ma:index="14" nillable="true" ma:displayName="Sharing Hint Hash" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE75B8BD-161F-4195-B4A2-4F1EFEFABD5B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fd496924-abde-4845-9207-bf2913a7250c"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5455B1F8-E48F-40D2-B780-CF700E136D16}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="fd496924-abde-4845-9207-bf2913a7250c"/>
+    <ds:schemaRef ds:uri="706ff326-42ab-42a4-bae8-1cee897fc7b9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14DA2B4D-9BEC-4222-83CD-08A8CB8B8082}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>